<commit_message>
Maybe I will love Rezonit
</commit_message>
<xml_diff>
--- a/Mainboard/Project Outputs for Mainboard/Folder Structure/Bill of Materials-Mainboard.xlsx
+++ b/Mainboard/Project Outputs for Mainboard/Folder Structure/Bill of Materials-Mainboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vlad\Documents\GitHub\CalibratorPCB\Mainboard\Project Outputs for Mainboard\Folder Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCED7D35-BC4D-44EE-A477-92E1DC7B30F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABA95C6B-B411-4D60-9343-8B90B841067A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="3795" windowWidth="21600" windowHeight="11385" xr2:uid="{E7A23027-3B20-4891-8F19-16F077FD9796}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{57C4826F-24EA-4BF8-BB22-9238C4BC68AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Mainboard" sheetId="1" r:id="rId1"/>
@@ -891,7 +891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BBBADC-E859-4CB8-BDB9-8D80F2E29F81}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A371DE-094B-4E4D-9BB4-2E4B5F3773A0}">
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Fixed slot hole type per Rezonit rqst
</commit_message>
<xml_diff>
--- a/Mainboard/Project Outputs for Mainboard/Folder Structure/Bill of Materials-Mainboard.xlsx
+++ b/Mainboard/Project Outputs for Mainboard/Folder Structure/Bill of Materials-Mainboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vlad\Documents\GitHub\CalibratorPCB\Mainboard\Project Outputs for Mainboard\Folder Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABA95C6B-B411-4D60-9343-8B90B841067A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C75B7796-631D-41EC-9426-C3E6BA261D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{57C4826F-24EA-4BF8-BB22-9238C4BC68AD}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{835A9A0D-54F3-4757-BA09-71D6DFAFB5DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Mainboard" sheetId="1" r:id="rId1"/>
@@ -891,7 +891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A371DE-094B-4E4D-9BB4-2E4B5F3773A0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4904515-646C-4227-BE8B-2999431A599F}">
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>